<commit_message>
Update of CO RSS
</commit_message>
<xml_diff>
--- a/_Excel/CO.xlsx
+++ b/_Excel/CO.xlsx
@@ -1,41 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bridge\City2223_SEM_A\EE3301\letcure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E68283-B57F-4822-A6CE-5F9EF8BD2035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129DA9A-6AA2-402F-A587-F6C26D6FF157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC2E2FC5-DA51-4960-A3F6-A09C52315A33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EC2E2FC5-DA51-4960-A3F6-A09C52315A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Convex  Opt." sheetId="1" r:id="rId1"/>
+    <sheet name="RSS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Convex  Opt.'!$A$11:$C$11</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">RSS!$E$2:$F$2</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Convex  Opt.'!$F$3:$F$7</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Convex  Opt.'!$M$3:$M$7</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Convex  Opt.'!$M$3:$M$7</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Convex  Opt.'!$E$11</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">RSS!$I$2</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
@@ -43,15 +61,25 @@
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Convex  Opt.'!$L$3:$L$7</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Convex  Opt.'!$L$3:$L$7</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>&lt;- modify function here</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -129,12 +157,63 @@
     <t>Subject to</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>xi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Slope</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ri^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum xi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum yi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sumsq xi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sumsq yi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum xiyi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,8 +273,15 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +306,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -549,13 +641,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -676,6 +867,108 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,8 +997,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{55E56BEF-24B8-45AD-B1F7-17C6D8039947}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1019,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3E2DE1-3E78-4D59-8881-BF2F12FA3F9A}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -1030,21 +1324,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="76"/>
     </row>
     <row r="2" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1232,16 +1526,16 @@
     </row>
     <row r="8" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="45"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -1276,11 +1570,11 @@
         <f>2-POWER(2,-A11)-POWER(50,-B11)</f>
         <v>1.5295355574114708</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="48"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="82"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
@@ -1293,4 +1587,495 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4E759D-B4E8-409F-B7F8-800F102C233E}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="9" style="46"/>
+    <col min="3" max="3" width="9" style="47"/>
+    <col min="4" max="4" width="2.625" customWidth="1"/>
+    <col min="5" max="5" width="9" style="46"/>
+    <col min="6" max="6" width="9" style="47"/>
+    <col min="7" max="7" width="2.625" customWidth="1"/>
+    <col min="8" max="9" width="9" style="44"/>
+    <col min="10" max="10" width="2.625" customWidth="1"/>
+    <col min="11" max="11" width="9" style="72"/>
+    <col min="12" max="12" width="9" style="50"/>
+    <col min="13" max="13" width="2.625" customWidth="1"/>
+    <col min="14" max="14" width="9" style="49"/>
+    <col min="15" max="15" width="9" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="43"/>
+      <c r="L1" s="45"/>
+      <c r="N1" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48">
+        <v>1</v>
+      </c>
+      <c r="B2" s="53">
+        <v>1.47</v>
+      </c>
+      <c r="C2" s="54">
+        <v>52.21</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="65">
+        <v>-39.059776148952594</v>
+      </c>
+      <c r="F2" s="66">
+        <v>61.270641147548424</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="63">
+        <f>POWER(C2-$E$2-$F$2*B2,2)</f>
+        <v>1.4446445279843196</v>
+      </c>
+      <c r="I2" s="57">
+        <f>SUM(H2:H21)</f>
+        <v>7.490560906610666</v>
+      </c>
+      <c r="K2" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="67">
+        <f>COUNTA(B2:B21)</f>
+        <v>15</v>
+      </c>
+      <c r="N2" s="58">
+        <f>(L4-O2*L3)/L2</f>
+        <v>-39.061955918838656</v>
+      </c>
+      <c r="O2" s="59">
+        <f>(L2*L7-L3*L4)/(L2*L5-POWER(L3,2))</f>
+        <v>61.272186542107434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="54">
+        <v>53.12</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="63">
+        <f t="shared" ref="H3:H16" si="0">POWER(C3-$E$2-$F$2*B3,2)</f>
+        <v>7.4974340778313664E-2</v>
+      </c>
+      <c r="I3" s="48"/>
+      <c r="K3" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="68">
+        <f>SUM(B2:B21)</f>
+        <v>24.759999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="48">
+        <v>3</v>
+      </c>
+      <c r="B4" s="53">
+        <v>1.52</v>
+      </c>
+      <c r="C4" s="54">
+        <v>54.48</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="63">
+        <f t="shared" si="0"/>
+        <v>0.1667918707043704</v>
+      </c>
+      <c r="I4" s="48"/>
+      <c r="K4" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="68">
+        <f>SUM(C2:C21)</f>
+        <v>931.17000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="53">
+        <v>1.55</v>
+      </c>
+      <c r="C5" s="54">
+        <v>55.84</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="63">
+        <f t="shared" si="0"/>
+        <v>4.8605478976037012E-3</v>
+      </c>
+      <c r="I5" s="48"/>
+      <c r="K5" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="68">
+        <f>SUMSQ(B2:B21)</f>
+        <v>41.053199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="48">
+        <v>5</v>
+      </c>
+      <c r="B6" s="53">
+        <v>1.57</v>
+      </c>
+      <c r="C6" s="54">
+        <v>57.2</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="63">
+        <f t="shared" si="0"/>
+        <v>4.2080581671105292E-3</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="K6" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="68">
+        <f>SUMSQ(C2:C21)</f>
+        <v>58498.543899999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48">
+        <v>6</v>
+      </c>
+      <c r="B7" s="53">
+        <v>1.6</v>
+      </c>
+      <c r="C7" s="54">
+        <v>58.57</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="63">
+        <f t="shared" si="0"/>
+        <v>0.16261031016631672</v>
+      </c>
+      <c r="I7" s="48"/>
+      <c r="K7" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="66">
+        <f>SUMPRODUCT(B2:B21,C2:C21)</f>
+        <v>1548.2452999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
+        <v>7</v>
+      </c>
+      <c r="B8" s="53">
+        <v>1.63</v>
+      </c>
+      <c r="C8" s="54">
+        <v>59.93</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="63">
+        <f t="shared" si="0"/>
+        <v>0.77681117587657578</v>
+      </c>
+      <c r="I8" s="48"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="48">
+        <v>8</v>
+      </c>
+      <c r="B9" s="53">
+        <v>1.65</v>
+      </c>
+      <c r="C9" s="54">
+        <v>61.29</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="63">
+        <f t="shared" si="0"/>
+        <v>0.55768297392189869</v>
+      </c>
+      <c r="I9" s="48"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="48">
+        <v>9</v>
+      </c>
+      <c r="B10" s="53">
+        <v>1.68</v>
+      </c>
+      <c r="C10" s="54">
+        <v>63.11</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="63">
+        <f t="shared" si="0"/>
+        <v>0.58507350756616072</v>
+      </c>
+      <c r="I10" s="48"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="48">
+        <v>10</v>
+      </c>
+      <c r="B11" s="53">
+        <v>1.7</v>
+      </c>
+      <c r="C11" s="54">
+        <v>64.47</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="63">
+        <f t="shared" si="0"/>
+        <v>0.39729548884007038</v>
+      </c>
+      <c r="I11" s="48"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="48">
+        <v>11</v>
+      </c>
+      <c r="B12" s="53">
+        <v>1.73</v>
+      </c>
+      <c r="C12" s="54">
+        <v>66.28</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="63">
+        <f t="shared" si="0"/>
+        <v>0.43353406329937288</v>
+      </c>
+      <c r="I12" s="48"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="48">
+        <v>12</v>
+      </c>
+      <c r="B13" s="53">
+        <v>1.75</v>
+      </c>
+      <c r="C13" s="54">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="63">
+        <f t="shared" si="0"/>
+        <v>4.0762937442846607E-3</v>
+      </c>
+      <c r="I13" s="48"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="48">
+        <v>13</v>
+      </c>
+      <c r="B14" s="53">
+        <v>1.78</v>
+      </c>
+      <c r="C14" s="54">
+        <v>69.92</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="63">
+        <f t="shared" si="0"/>
+        <v>6.7182765825624623E-3</v>
+      </c>
+      <c r="I14" s="48"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="48">
+        <v>14</v>
+      </c>
+      <c r="B15" s="53">
+        <v>1.8</v>
+      </c>
+      <c r="C15" s="54">
+        <v>72.19</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="63">
+        <f t="shared" si="0"/>
+        <v>0.92664127538280383</v>
+      </c>
+      <c r="I15" s="48"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="48">
+        <v>15</v>
+      </c>
+      <c r="B16" s="53">
+        <v>1.83</v>
+      </c>
+      <c r="C16" s="54">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="63">
+        <f t="shared" si="0"/>
+        <v>1.9446381956989036</v>
+      </c>
+      <c r="I16" s="48"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="48">
+        <v>16</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="48"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="48">
+        <v>17</v>
+      </c>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="48"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="48">
+        <v>18</v>
+      </c>
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="48"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="48">
+        <v>19</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="48"/>
+    </row>
+    <row r="21" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="51">
+        <v>20</v>
+      </c>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="40"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on organising LP and CO excel
</commit_message>
<xml_diff>
--- a/_Excel/CO.xlsx
+++ b/_Excel/CO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bridge\City2223_SEM_A\EE3301\letcure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129DA9A-6AA2-402F-A587-F6C26D6FF157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6075113E-21F4-44FF-A97E-00EB78695F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EC2E2FC5-DA51-4960-A3F6-A09C52315A33}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Convex  Opt.'!$A$11:$C$11</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">RSS!$E$2:$F$2</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">RSS!$F$2:$G$2</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
@@ -49,7 +49,7 @@
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Convex  Opt.'!$E$11</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">RSS!$I$2</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">RSS!$E$2</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>&lt;- modify function here</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -154,10 +154,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Subject to</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>xi</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -206,6 +202,17 @@
   </si>
   <si>
     <t>n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>%err</t>
+  </si>
+  <si>
+    <t>%err</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Such that</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -281,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,8 +319,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -720,19 +733,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -746,7 +746,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,7 +900,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -918,13 +918,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -939,7 +933,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,25 +942,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -994,6 +982,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1317,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1324,21 +1327,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="76"/>
+      <c r="A1" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="72"/>
     </row>
     <row r="2" spans="1:13" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1526,16 +1529,16 @@
     </row>
     <row r="8" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="79"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -1570,11 +1573,11 @@
         <f>2-POWER(2,-A11)-POWER(50,-B11)</f>
         <v>1.5295355574114708</v>
       </c>
-      <c r="F11" s="80" t="s">
+      <c r="F11" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="81"/>
-      <c r="H11" s="82"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="78"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
@@ -1594,7 +1597,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1602,51 +1605,50 @@
     <col min="1" max="1" width="4.625" style="44" customWidth="1"/>
     <col min="2" max="2" width="9" style="46"/>
     <col min="3" max="3" width="9" style="47"/>
-    <col min="4" max="4" width="2.625" customWidth="1"/>
-    <col min="5" max="5" width="9" style="46"/>
-    <col min="6" max="6" width="9" style="47"/>
-    <col min="7" max="7" width="2.625" customWidth="1"/>
-    <col min="8" max="9" width="9" style="44"/>
-    <col min="10" max="10" width="2.625" customWidth="1"/>
-    <col min="11" max="11" width="9" style="72"/>
-    <col min="12" max="12" width="9" style="50"/>
-    <col min="13" max="13" width="2.625" customWidth="1"/>
-    <col min="14" max="14" width="9" style="49"/>
-    <col min="15" max="15" width="9" style="50"/>
+    <col min="4" max="5" width="9" style="44"/>
+    <col min="6" max="6" width="10.625" style="46" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="47" customWidth="1"/>
+    <col min="8" max="8" width="2.625" customWidth="1"/>
+    <col min="9" max="9" width="9" style="68"/>
+    <col min="10" max="10" width="9" style="50"/>
+    <col min="11" max="11" width="2.625" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="49" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="50" customWidth="1"/>
+    <col min="14" max="15" width="10.625" style="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="42" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="45" t="s">
+      <c r="E1" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="G1" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="45"/>
-      <c r="N1" s="61" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="45"/>
+      <c r="L1" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -1656,39 +1658,39 @@
       <c r="C2" s="54">
         <v>52.21</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="65">
-        <v>-39.059776148952594</v>
-      </c>
-      <c r="F2" s="66">
-        <v>61.270641147548424</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="63">
-        <f>POWER(C2-$E$2-$F$2*B2,2)</f>
-        <v>1.4446445279843196</v>
-      </c>
-      <c r="I2" s="57">
-        <f>SUM(H2:H21)</f>
-        <v>7.490560906610666</v>
-      </c>
-      <c r="K2" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="67">
+      <c r="D2" s="61">
+        <f>POWER(C2-$F$2-$G$2*B2,2)</f>
+        <v>1.4438169818392723</v>
+      </c>
+      <c r="E2" s="57">
+        <f>SUM(D2:D21)</f>
+        <v>7.4905587378564178</v>
+      </c>
+      <c r="F2" s="63">
+        <v>-39.059719252840253</v>
+      </c>
+      <c r="G2" s="64">
+        <v>61.270836664124616</v>
+      </c>
+      <c r="H2" s="79"/>
+      <c r="I2" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="65">
         <f>COUNTA(B2:B21)</f>
         <v>15</v>
       </c>
-      <c r="N2" s="58">
-        <f>(L4-O2*L3)/L2</f>
+      <c r="K2" s="80"/>
+      <c r="L2" s="63">
+        <f>(J4-M2*J3)/J2</f>
         <v>-39.061955918838656</v>
       </c>
-      <c r="O2" s="59">
-        <f>(L2*L7-L3*L4)/(L2*L5-POWER(L3,2))</f>
+      <c r="M2" s="64">
+        <f>(J2*J7-J3*J4)/(J2*J5-POWER(J3,2))</f>
         <v>61.272186542107434</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -1698,24 +1700,30 @@
       <c r="C3" s="54">
         <v>53.12</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="63">
-        <f t="shared" ref="H3:H16" si="0">POWER(C3-$E$2-$F$2*B3,2)</f>
-        <v>7.4974340778313664E-2</v>
-      </c>
-      <c r="I3" s="48"/>
-      <c r="K3" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="68">
+      <c r="D3" s="61">
+        <f>POWER(C3-$F$2-$G$2*B3,2)</f>
+        <v>7.4782699666948782E-2</v>
+      </c>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="65">
         <f>SUM(B2:B21)</f>
         <v>24.759999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3" s="80"/>
+      <c r="L3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -1725,24 +1733,32 @@
       <c r="C4" s="54">
         <v>54.48</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="63">
-        <f t="shared" si="0"/>
-        <v>0.1667918707043704</v>
-      </c>
-      <c r="I4" s="48"/>
-      <c r="K4" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="68">
+      <c r="D4" s="61">
+        <f>POWER(C4-$F$2-$G$2*B4,2)</f>
+        <v>0.16650278132907606</v>
+      </c>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="65">
         <f>SUM(C2:C21)</f>
         <v>931.17000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4" s="80"/>
+      <c r="L4" s="81">
+        <f>(L2-F2)/L2*100</f>
+        <v>5.7259447096050476E-3</v>
+      </c>
+      <c r="M4" s="82">
+        <f>(M2-G2)/M2*100</f>
+        <v>2.2030843992985436E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>4</v>
       </c>
@@ -1752,24 +1768,24 @@
       <c r="C5" s="54">
         <v>55.84</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="63">
-        <f t="shared" si="0"/>
-        <v>4.8605478976037012E-3</v>
-      </c>
-      <c r="I5" s="48"/>
-      <c r="K5" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="68">
+      <c r="D5" s="61">
+        <f>POWER(C5-$F$2-$G$2*B5,2)</f>
+        <v>4.9108667355281868E-3</v>
+      </c>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="65">
         <f>SUMSQ(B2:B21)</f>
         <v>41.053199999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>5</v>
       </c>
@@ -1779,24 +1795,24 @@
       <c r="C6" s="54">
         <v>57.2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="63">
-        <f t="shared" si="0"/>
-        <v>4.2080581671105292E-3</v>
-      </c>
-      <c r="I6" s="48"/>
-      <c r="K6" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="68">
+      <c r="D6" s="61">
+        <f>POWER(C6-$F$2-$G$2*B6,2)</f>
+        <v>4.1609840636124837E-3</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="83">
         <f>SUMSQ(C2:C21)</f>
         <v>58498.543899999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="80"/>
+    </row>
+    <row r="7" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48">
         <v>6</v>
       </c>
@@ -1806,24 +1822,24 @@
       <c r="C7" s="54">
         <v>58.57</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="63">
-        <f t="shared" si="0"/>
-        <v>0.16261031016631672</v>
-      </c>
-      <c r="I7" s="48"/>
-      <c r="K7" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="66">
+      <c r="D7" s="61">
+        <f>POWER(C7-$F$2-$G$2*B7,2)</f>
+        <v>0.16290862793430896</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="64">
         <f>SUMPRODUCT(B2:B21,C2:C21)</f>
         <v>1548.2452999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="80"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>7</v>
       </c>
@@ -1833,17 +1849,17 @@
       <c r="C8" s="54">
         <v>59.93</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="63">
-        <f t="shared" si="0"/>
-        <v>0.77681117587657578</v>
-      </c>
-      <c r="I8" s="48"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D8" s="61">
+        <f>POWER(C8-$F$2-$G$2*B8,2)</f>
+        <v>0.77747338035589342</v>
+      </c>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="79"/>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>8</v>
       </c>
@@ -1853,17 +1869,17 @@
       <c r="C9" s="54">
         <v>61.29</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="63">
-        <f t="shared" si="0"/>
-        <v>0.55768297392189869</v>
-      </c>
-      <c r="I9" s="48"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="61">
+        <f>POWER(C9-$F$2-$G$2*B9,2)</f>
+        <v>0.55824992298952314</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="79"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>9</v>
       </c>
@@ -1873,17 +1889,17 @@
       <c r="C10" s="54">
         <v>63.11</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="63">
-        <f t="shared" si="0"/>
-        <v>0.58507350756616072</v>
-      </c>
-      <c r="I10" s="48"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="61">
+        <f>POWER(C10-$F$2-$G$2*B10,2)</f>
+        <v>0.58566318661257033</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="79"/>
+      <c r="K10" s="80"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>10</v>
       </c>
@@ -1893,17 +1909,17 @@
       <c r="C11" s="54">
         <v>64.47</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="63">
-        <f t="shared" si="0"/>
-        <v>0.39729548884007038</v>
-      </c>
-      <c r="I11" s="48"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="61">
+        <f>POWER(C11-$F$2-$G$2*B11,2)</f>
+        <v>0.39778637029231817</v>
+      </c>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="79"/>
+      <c r="K11" s="80"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <v>11</v>
       </c>
@@ -1913,17 +1929,17 @@
       <c r="C12" s="54">
         <v>66.28</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="63">
-        <f t="shared" si="0"/>
-        <v>0.43353406329937288</v>
-      </c>
-      <c r="I12" s="48"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="61">
+        <f>POWER(C12-$F$2-$G$2*B12,2)</f>
+        <v>0.43405456561709455</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="79"/>
+      <c r="K12" s="80"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>12</v>
       </c>
@@ -1933,17 +1949,17 @@
       <c r="C13" s="54">
         <v>68.099999999999994</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="63">
-        <f t="shared" si="0"/>
-        <v>4.0762937442846607E-3</v>
-      </c>
-      <c r="I13" s="48"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="61">
+        <f>POWER(C13-$F$2-$G$2*B13,2)</f>
+        <v>4.1274083809660893E-3</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="79"/>
+      <c r="K13" s="80"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>13</v>
       </c>
@@ -1953,17 +1969,17 @@
       <c r="C14" s="54">
         <v>69.92</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="63">
-        <f t="shared" si="0"/>
-        <v>6.7182765825624623E-3</v>
-      </c>
-      <c r="I14" s="48"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" s="61">
+        <f>POWER(C14-$F$2-$G$2*B14,2)</f>
+        <v>6.7848184323384261E-3</v>
+      </c>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="79"/>
+      <c r="K14" s="80"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>14</v>
       </c>
@@ -1973,17 +1989,17 @@
       <c r="C15" s="54">
         <v>72.19</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="63">
-        <f t="shared" si="0"/>
-        <v>0.92664127538280383</v>
-      </c>
-      <c r="I15" s="48"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D15" s="61">
+        <f>POWER(C15-$F$2-$G$2*B15,2)</f>
+        <v>0.9258543527469929</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="79"/>
+      <c r="K15" s="80"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <v>15</v>
       </c>
@@ -1993,86 +2009,84 @@
       <c r="C16" s="54">
         <v>74.459999999999994</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="63">
-        <f t="shared" si="0"/>
-        <v>1.9446381956989036</v>
-      </c>
-      <c r="I16" s="48"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D16" s="61">
+        <f>POWER(C16-$F$2-$G$2*B16,2)</f>
+        <v>1.943481790859974</v>
+      </c>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="79"/>
+      <c r="K16" s="80"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <v>16</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="48"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="61"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="79"/>
+      <c r="K17" s="80"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>17</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="54"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="48"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="61"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="79"/>
+      <c r="K18" s="80"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <v>18</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="54"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="48"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D19" s="61"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="79"/>
+      <c r="K19" s="80"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <v>19</v>
       </c>
       <c r="B20" s="53"/>
       <c r="C20" s="54"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="48"/>
-    </row>
-    <row r="21" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="61"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="79"/>
+      <c r="K20" s="80"/>
+    </row>
+    <row r="21" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="51">
         <v>20</v>
       </c>
       <c r="B21" s="55"/>
       <c r="C21" s="56"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="40"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="40"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>